<commit_message>
CPR Pharmacy files updated
Chenges in contact sequence dropdown
</commit_message>
<xml_diff>
--- a/QA/testcases/CPR/Pharmacy/Phar_Patient_App_Create_PCase_Positive.xlsx
+++ b/QA/testcases/CPR/Pharmacy/Phar_Patient_App_Create_PCase_Positive.xlsx
@@ -1,43 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\fipsar_automation\QA\testcases\CPR\Pharmacy\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63CFEDD5-C839-45EA-8E81-6CEF365A7A97}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28680" windowHeight="13650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="20385" windowHeight="7740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="DataList" sheetId="3" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
     <externalReference r:id="rId4"/>
     <externalReference r:id="rId5"/>
     <externalReference r:id="rId6"/>
     <externalReference r:id="rId7"/>
     <externalReference r:id="rId8"/>
+    <externalReference r:id="rId9"/>
   </externalReferences>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="Rewards" type="5" refreshedVersion="2" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="Rewards" type="5" background="1" refreshedVersion="2" saveData="1">
     <dbPr connection="Provider=Microsoft.ACE.OLEDB.12.0;Password=&quot;&quot;;User ID=Admin;Data Source=C:\Framework\testcase\Crowd\Rewards.xlsx;Mode=Share Deny Write;Extended Properties=&quot;HDR=YES;&quot;;Jet OLEDB:System database=&quot;&quot;;Jet OLEDB:Registry Path=&quot;&quot;;Jet OLEDB:Database Password=&quot;&quot;;Jet OLEDB:Engine Type=37;Jet OLEDB:Database Locking Mode=0;Jet OLEDB:Global Partial Bulk Ops=2;Jet OLEDB:Global Bulk Transactions=1;Jet OLEDB:New Database Password=&quot;&quot;;Jet OLEDB:Create System Database=False;Jet OLEDB:Encrypt Database=False;Jet OLEDB:Don't Copy Locale on Compact=False;Jet OLEDB:Compact Without Replica Repair=False;Jet OLEDB:SFP=False;Jet OLEDB:Support Complex Data=False" command="DataList$" commandType="3"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405">
   <si>
     <t>Step No</t>
   </si>
@@ -387,6 +381,9 @@
     <t>CONTACT_PNONE_NUMBER</t>
   </si>
   <si>
+    <t>SelectByIndex</t>
+  </si>
+  <si>
     <t>CONTACT_SEQUENCE</t>
   </si>
   <si>
@@ -1047,9 +1044,6 @@
     <t>SelectCheckBox</t>
   </si>
   <si>
-    <t>SelectByIndex</t>
-  </si>
-  <si>
     <t>SelectByValue</t>
   </si>
   <si>
@@ -1252,16 +1246,19 @@
   </si>
   <si>
     <t>SikuliClick</t>
-  </si>
-  <si>
-    <t>Primary</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1285,8 +1282,152 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1301,12 +1442,198 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79995117038483843"/>
-        <bgColor theme="4" tint="0.79995117038483843"/>
+        <fgColor theme="4" tint="0.799951170384838"/>
+        <bgColor theme="4" tint="0.799951170384838"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1316,16 +1643,16 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="4" tint="0.39982299264503923"/>
+        <color theme="4" tint="0.399822992645039"/>
       </left>
       <right style="thin">
-        <color theme="4" tint="0.39982299264503923"/>
+        <color theme="4" tint="0.399822992645039"/>
       </right>
       <top style="thin">
-        <color theme="4" tint="0.39982299264503923"/>
+        <color theme="4" tint="0.399822992645039"/>
       </top>
       <bottom style="thin">
-        <color theme="4" tint="0.39982299264503923"/>
+        <color theme="4" tint="0.399822992645039"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1333,10 +1660,10 @@
       <left/>
       <right/>
       <top style="thin">
-        <color theme="4" tint="0.39991454817346722"/>
+        <color theme="4" tint="0.399914548173467"/>
       </top>
       <bottom style="thin">
-        <color theme="4" tint="0.39991454817346722"/>
+        <color theme="4" tint="0.399914548173467"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1344,16 +1671,258 @@
       <left/>
       <right/>
       <top style="thin">
-        <color theme="4" tint="0.39994506668294322"/>
+        <color theme="4" tint="0.399945066682943"/>
       </top>
       <bottom style="thin">
-        <color theme="4" tint="0.39994506668294322"/>
+        <color theme="4" tint="0.399945066682943"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1365,24 +1934,68 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Xpath"/>
@@ -1397,7 +2010,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
@@ -1412,7 +2025,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
@@ -1427,7 +2040,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
@@ -1442,7 +2055,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
@@ -1457,7 +2070,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
@@ -1472,18 +2085,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:A13" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:A13" totalsRowShown="0">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="LocateBy"/>
+    <tableColumn id="1" name="LocateBy"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table3" displayName="Table3" ref="C1:C101" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="C1:C101" totalsRowShown="0">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Actions"/>
+    <tableColumn id="1" name="Actions"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1741,29 +2354,29 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:H156"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85714285714286" defaultRowHeight="15" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="87.7109375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="33.28515625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" style="4" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="4"/>
+    <col min="1" max="1" width="8.57142857142857" style="4" customWidth="1"/>
+    <col min="2" max="2" width="24.2857142857143" style="4" customWidth="1"/>
+    <col min="3" max="3" width="9.42857142857143" style="4" customWidth="1"/>
+    <col min="4" max="4" width="28.1428571428571" style="4" customWidth="1"/>
+    <col min="5" max="5" width="19.4285714285714" style="4" customWidth="1"/>
+    <col min="6" max="6" width="87.7142857142857" style="4" customWidth="1"/>
+    <col min="7" max="7" width="33.2857142857143" style="4" customWidth="1"/>
+    <col min="8" max="8" width="15.7142857142857" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="8.85714285714286" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -2691,16 +3304,16 @@
         <v>42</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>42</v>
+        <v>116</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>405</v>
+        <v>117</v>
+      </c>
+      <c r="E43" s="7">
+        <v>1</v>
       </c>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
@@ -2759,7 +3372,7 @@
         <v>20</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
@@ -2777,13 +3390,13 @@
         <v>15</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G47" s="7" t="s">
         <v>28</v>
@@ -2801,13 +3414,13 @@
         <v>15</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G48" s="6" t="s">
         <v>32</v>
@@ -2825,16 +3438,16 @@
         <v>20</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H49" s="7"/>
     </row>
@@ -2849,16 +3462,16 @@
         <v>15</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H50" s="6"/>
     </row>
@@ -2873,13 +3486,13 @@
         <v>20</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E51" s="7" t="s">
         <v>101</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G51" s="7" t="s">
         <v>103</v>
@@ -2897,13 +3510,13 @@
         <v>15</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E52" s="6" t="s">
         <v>105</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G52" s="6" t="s">
         <v>107</v>
@@ -2921,16 +3534,16 @@
         <v>15</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E53" s="7">
         <v>10001</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H53" s="7"/>
     </row>
@@ -2945,16 +3558,16 @@
         <v>15</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E54" s="6">
         <v>9789123456</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H54" s="6"/>
     </row>
@@ -2969,16 +3582,16 @@
         <v>15</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H55" s="7"/>
     </row>
@@ -3035,16 +3648,16 @@
         <v>20</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H58" s="6"/>
     </row>
@@ -3069,16 +3682,16 @@
         <v>59</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C60" s="6"/>
       <c r="D60" s="6"/>
       <c r="E60" s="6"/>
       <c r="F60" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H60" s="6"/>
     </row>
@@ -3093,16 +3706,16 @@
         <v>20</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F61" s="7" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G61" s="7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H61" s="7"/>
     </row>
@@ -3117,16 +3730,16 @@
         <v>15</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H62" s="6"/>
     </row>
@@ -3141,16 +3754,16 @@
         <v>20</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G63" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H63" s="7"/>
     </row>
@@ -3165,16 +3778,16 @@
         <v>15</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E64" s="6" t="s">
         <v>97</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H64" s="6"/>
     </row>
@@ -3189,16 +3802,16 @@
         <v>15</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E65" s="7">
         <v>1235647899</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G65" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H65" s="7"/>
     </row>
@@ -3213,7 +3826,7 @@
         <v>20</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E66" s="6"/>
       <c r="F66" s="6"/>
@@ -3231,14 +3844,14 @@
         <v>20</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E67" s="7"/>
       <c r="F67" s="7" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="G67" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H67" s="7"/>
     </row>
@@ -3253,16 +3866,16 @@
         <v>15</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E68" s="6">
         <v>97890456789</v>
       </c>
       <c r="F68" s="6" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H68" s="6"/>
     </row>
@@ -3277,14 +3890,14 @@
         <v>20</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E69" s="7"/>
       <c r="F69" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G69" s="7" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H69" s="7"/>
     </row>
@@ -3299,16 +3912,16 @@
         <v>20</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E70" s="6">
         <v>1230</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H70" s="6"/>
     </row>
@@ -3323,16 +3936,16 @@
         <v>20</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E71" s="7">
         <v>1550</v>
       </c>
       <c r="F71" s="7" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G71" s="7" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H71" s="7"/>
     </row>
@@ -3347,14 +3960,14 @@
         <v>20</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E72" s="6"/>
       <c r="F72" s="6" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="G72" s="6" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H72" s="6"/>
     </row>
@@ -3369,14 +3982,14 @@
         <v>20</v>
       </c>
       <c r="D73" s="7" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E73" s="7"/>
       <c r="F73" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="G73" s="7" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H73" s="7"/>
     </row>
@@ -3391,14 +4004,14 @@
         <v>20</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E74" s="6"/>
       <c r="F74" s="6" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H74" s="6"/>
     </row>
@@ -3413,14 +4026,14 @@
         <v>20</v>
       </c>
       <c r="D75" s="7" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E75" s="7"/>
       <c r="F75" s="7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="G75" s="7" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H75" s="7"/>
     </row>
@@ -3477,7 +4090,7 @@
         <v>20</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E78" s="6"/>
       <c r="F78" s="6"/>
@@ -3537,16 +4150,16 @@
         <v>20</v>
       </c>
       <c r="D81" s="7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E81" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F81" s="7" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="G81" s="7" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="H81" s="7"/>
     </row>
@@ -3571,16 +4184,16 @@
         <v>82</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C83" s="7"/>
       <c r="D83" s="7"/>
       <c r="E83" s="7"/>
       <c r="F83" s="7" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G83" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="H83" s="7"/>
     </row>
@@ -3595,14 +4208,14 @@
         <v>20</v>
       </c>
       <c r="D84" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E84" s="6"/>
       <c r="F84" s="6" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="G84" s="6" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="H84" s="6"/>
     </row>
@@ -3617,14 +4230,14 @@
         <v>20</v>
       </c>
       <c r="D85" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E85" s="7"/>
       <c r="F85" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="G85" s="7" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="H85" s="7"/>
     </row>
@@ -3681,14 +4294,14 @@
         <v>20</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E88" s="6"/>
       <c r="F88" s="6" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="G88" s="6" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="H88" s="6"/>
     </row>
@@ -3719,7 +4332,7 @@
         <v>20</v>
       </c>
       <c r="D90" s="6" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E90" s="6"/>
       <c r="F90" s="6"/>
@@ -3753,14 +4366,14 @@
         <v>20</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E92" s="6"/>
       <c r="F92" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="G92" s="6" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="H92" s="6"/>
     </row>
@@ -3777,10 +4390,10 @@
         <v>3</v>
       </c>
       <c r="F93" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="G93" s="7" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="H93" s="7"/>
     </row>
@@ -3795,14 +4408,14 @@
         <v>20</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E94" s="6"/>
       <c r="F94" s="6" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G94" s="6" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H94" s="6"/>
     </row>
@@ -3817,14 +4430,14 @@
         <v>20</v>
       </c>
       <c r="D95" s="7" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E95" s="7"/>
       <c r="F95" s="7" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G95" s="7" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H95" s="7"/>
     </row>
@@ -3855,16 +4468,16 @@
         <v>15</v>
       </c>
       <c r="D97" s="7" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E97" s="7" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="F97" s="7" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G97" s="7" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="H97" s="7"/>
     </row>
@@ -3879,16 +4492,16 @@
         <v>15</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E98" s="6" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F98" s="6" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G98" s="6" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H98" s="6"/>
     </row>
@@ -3903,16 +4516,16 @@
         <v>15</v>
       </c>
       <c r="D99" s="7" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E99" s="7">
         <v>9889656446</v>
       </c>
       <c r="F99" s="7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G99" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H99" s="7"/>
     </row>
@@ -3927,14 +4540,14 @@
         <v>15</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E100" s="6"/>
       <c r="F100" s="6" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G100" s="6" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="H100" s="6"/>
     </row>
@@ -3963,20 +4576,20 @@
         <v>101</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C102" s="6" t="s">
         <v>20</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E102" s="6"/>
       <c r="F102" s="6" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="G102" s="6" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="H102" s="6"/>
     </row>
@@ -3985,20 +4598,20 @@
         <v>102</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C103" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D103" s="7" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E103" s="7"/>
       <c r="F103" s="7" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G103" s="7" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="H103" s="7"/>
     </row>
@@ -4007,20 +4620,20 @@
         <v>103</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C104" s="6" t="s">
         <v>20</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E104" s="6"/>
       <c r="F104" s="6" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="G104" s="6" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="H104" s="6"/>
     </row>
@@ -4029,20 +4642,20 @@
         <v>104</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C105" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D105" s="7" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E105" s="7"/>
       <c r="F105" s="7" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="G105" s="7" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="H105" s="7"/>
     </row>
@@ -4051,20 +4664,20 @@
         <v>105</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C106" s="6" t="s">
         <v>20</v>
       </c>
       <c r="D106" s="6" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E106" s="6"/>
       <c r="F106" s="6" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="G106" s="6" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="H106" s="6"/>
     </row>
@@ -4073,20 +4686,20 @@
         <v>106</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C107" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D107" s="7" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E107" s="7"/>
       <c r="F107" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="G107" s="7" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="H107" s="7"/>
     </row>
@@ -4095,20 +4708,20 @@
         <v>107</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C108" s="6" t="s">
         <v>20</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="E108" s="6"/>
       <c r="F108" s="6" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="G108" s="6" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="H108" s="6"/>
     </row>
@@ -4117,20 +4730,20 @@
         <v>108</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C109" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D109" s="7" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E109" s="7"/>
       <c r="F109" s="7" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="G109" s="7" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="H109" s="7"/>
     </row>
@@ -4145,14 +4758,14 @@
         <v>20</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E110" s="6"/>
       <c r="F110" s="6" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="G110" s="6" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="H110" s="6"/>
     </row>
@@ -4245,14 +4858,14 @@
         <v>20</v>
       </c>
       <c r="D115" s="7" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E115" s="7"/>
       <c r="F115" s="7" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="G115" s="7" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="H115" s="7"/>
     </row>
@@ -4267,14 +4880,14 @@
         <v>15</v>
       </c>
       <c r="D116" s="6" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E116" s="6"/>
       <c r="F116" s="6" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="G116" s="6" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="H116" s="6"/>
     </row>
@@ -4305,14 +4918,14 @@
         <v>20</v>
       </c>
       <c r="D118" s="6" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="E118" s="6"/>
       <c r="F118" s="6" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="G118" s="6" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="H118" s="6"/>
     </row>
@@ -4327,16 +4940,16 @@
         <v>15</v>
       </c>
       <c r="D119" s="7" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E119" s="7" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="F119" s="7" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="G119" s="7" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="H119" s="7"/>
     </row>
@@ -4351,16 +4964,16 @@
         <v>20</v>
       </c>
       <c r="D120" s="6" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="E120" s="6" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F120" s="6" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="G120" s="6" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="H120" s="6"/>
     </row>
@@ -4369,22 +4982,22 @@
         <v>120</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C121" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D121" s="7" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="E121" s="7" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="F121" s="7" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="G121" s="7" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="H121" s="7"/>
     </row>
@@ -4403,10 +5016,10 @@
       </c>
       <c r="E122" s="6"/>
       <c r="F122" s="6" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="G122" s="6" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="H122" s="6"/>
     </row>
@@ -4435,7 +5048,7 @@
         <v>123</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C124" s="6"/>
       <c r="D124" s="6"/>
@@ -4475,14 +5088,14 @@
         <v>15</v>
       </c>
       <c r="D126" s="6" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="E126" s="6"/>
       <c r="F126" s="6" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="G126" s="6" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="H126" s="6"/>
     </row>
@@ -4513,7 +5126,7 @@
         <v>15</v>
       </c>
       <c r="D128" s="6" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="E128" s="6"/>
       <c r="F128" s="6"/>
@@ -4571,14 +5184,14 @@
         <v>20</v>
       </c>
       <c r="D131" s="7" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E131" s="7"/>
       <c r="F131" s="7" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="G131" s="7" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="H131" s="7"/>
     </row>
@@ -4593,14 +5206,14 @@
         <v>15</v>
       </c>
       <c r="D132" s="6" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="E132" s="6"/>
       <c r="F132" s="6" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="G132" s="6" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="H132" s="6"/>
     </row>
@@ -4631,14 +5244,14 @@
         <v>20</v>
       </c>
       <c r="D134" s="6" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E134" s="6"/>
       <c r="F134" s="6" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="G134" s="6" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="H134" s="6"/>
     </row>
@@ -4669,7 +5282,7 @@
         <v>20</v>
       </c>
       <c r="D136" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E136" s="6"/>
       <c r="F136" s="6"/>
@@ -4687,14 +5300,14 @@
         <v>20</v>
       </c>
       <c r="D137" s="7" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="E137" s="7"/>
       <c r="F137" s="7" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="G137" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H137" s="7"/>
     </row>
@@ -4709,7 +5322,7 @@
         <v>20</v>
       </c>
       <c r="D138" s="6" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="E138" s="6"/>
       <c r="F138" s="6"/>
@@ -4727,14 +5340,14 @@
         <v>20</v>
       </c>
       <c r="D139" s="7" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E139" s="7"/>
       <c r="F139" s="7" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="G139" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H139" s="7"/>
     </row>
@@ -4749,7 +5362,7 @@
         <v>20</v>
       </c>
       <c r="D140" s="6" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="E140" s="6">
         <v>200</v>
@@ -4769,7 +5382,7 @@
         <v>20</v>
       </c>
       <c r="D141" s="7" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="E141" s="7"/>
       <c r="F141" s="7" t="s">
@@ -4807,10 +5420,10 @@
         <v>15</v>
       </c>
       <c r="D143" s="7" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E143" s="7" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="F143" s="7"/>
       <c r="G143" s="7"/>
@@ -4821,22 +5434,22 @@
         <v>143</v>
       </c>
       <c r="B144" s="6" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C144" s="6" t="s">
         <v>20</v>
       </c>
       <c r="D144" s="6" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="E144" s="6" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="F144" s="6" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="G144" s="6" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="H144" s="6"/>
     </row>
@@ -4851,7 +5464,7 @@
         <v>20</v>
       </c>
       <c r="D145" s="7" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="E145" s="7"/>
       <c r="F145" s="7" t="s">
@@ -4889,7 +5502,7 @@
         <v>20</v>
       </c>
       <c r="D147" s="7" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E147" s="7"/>
       <c r="F147" s="7"/>
@@ -4907,7 +5520,7 @@
         <v>20</v>
       </c>
       <c r="D148" s="6" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="E148" s="6" t="s">
         <v>97</v>
@@ -4927,7 +5540,7 @@
         <v>20</v>
       </c>
       <c r="D149" s="7" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E149" s="7"/>
       <c r="F149" s="7"/>
@@ -4955,16 +5568,16 @@
         <v>150</v>
       </c>
       <c r="B151" s="7" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C151" s="7"/>
       <c r="D151" s="7"/>
       <c r="E151" s="7"/>
       <c r="F151" s="7" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="G151" s="7" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="H151" s="7"/>
     </row>
@@ -4989,20 +5602,20 @@
         <v>152</v>
       </c>
       <c r="B153" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C153" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D153" s="7" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="E153" s="7"/>
       <c r="F153" s="7" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="G153" s="7" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="H153" s="7"/>
     </row>
@@ -5011,20 +5624,20 @@
         <v>153</v>
       </c>
       <c r="B154" s="6" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C154" s="6" t="s">
         <v>20</v>
       </c>
       <c r="D154" s="6" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="E154" s="6"/>
       <c r="F154" s="6" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="G154" s="6" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="H154" s="6"/>
     </row>
@@ -5039,14 +5652,14 @@
         <v>20</v>
       </c>
       <c r="D155" s="7" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="E155" s="7"/>
       <c r="F155" s="7" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="G155" s="7" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="H155" s="7"/>
     </row>
@@ -5067,266 +5680,246 @@
       <c r="H156" s="6"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B93 B94 B112 C128 C130 B1:B3 B16:B36 B37:B85 B86:B91 B96:B111 B115:B128 B129:B131 B155:B156 C2:C3" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+  <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1">
+      <formula1>[1]DataList!#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4 C5 C6 C10 C11 C12 C112 B113 C113 B114 C114 B4:B12 B13:B15 C7:C9 C13:C15">
+      <formula1>[2]DataList!#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C44 C56 C79 C27:C33">
+      <formula1>[3]DataList!#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C76">
+      <formula1>[4]DataList!#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B93 B94 B112 C128 C130 B1:B3 B16:B36 B37:B85 B86:B91 B96:B111 B115:B128 B129:B131 B155:B156 C2:C3">
+      <formula1/>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C129 C16:C26">
+      <formula1>[5]DataList!#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B132:B135 B136:B154">
+      <formula1>[6]DataList!#REF!</formula1>
+    </dataValidation>
   </dataValidations>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
-          <x14:formula1>
-            <xm:f>'C:\workspace\qa-automation\qa-automation\Zillion\testcases\Quick Start\Enrollment\[QS_Enrollment_EmailAndPasswordPageFieldValidations.xlsx]DataList'!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>C1</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
-          <x14:formula1>
-            <xm:f>'C:\workspace\fipsar_automation\QA\testcases\CPR\Pharmacy\[Phar_Patient_App_ViewIncomplete -ok.xlsx]DataList'!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>C4 C5 C6 C10 C11 C12 C112 B113 C113 B114 C114 B4:B12 B13:B15 C7:C9 C13:C15</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
-          <x14:formula1>
-            <xm:f>'C:\workspace\fipsar_automation\QA\testcases\Patient\[PatientApplication_Process_Positive.xlsx]DataList'!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>C44 C56 C79 C27:C33</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
-          <x14:formula1>
-            <xm:f>'C:\workspace\fipsar_automation\QA\testcases\Patient\[PatientApplication_Process_Positive_PCase.xlsx]DataList'!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>C76</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000005000000}">
-          <x14:formula1>
-            <xm:f>'C:\workspace\fipsar_automation\QA\testcases\Patient\[Patient_Registration_Positive.xlsx]DataList'!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>C129 C16:C26</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000006000000}">
-          <x14:formula1>
-            <xm:f>'C:\workspace\fipsar_automation\QA\testcases\Patient\[PatientApp_Process_Positive_PCase_Yes.xlsx]DataList'!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>B132:B135 B136:B154</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85714285714286" defaultRowHeight="15" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="3" max="3" width="52.5703125" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.5714285714286" customWidth="1"/>
+    <col min="3" max="3" width="52.5714285714286" customWidth="1"/>
+    <col min="4" max="4" width="13.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C3" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C6" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C8" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C10" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C11" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="12" spans="3:3">
       <c r="C12" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="13" spans="3:3">
       <c r="C13" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="14" spans="3:3">
       <c r="C14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="3:3">
       <c r="C15" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="16" spans="3:3">
       <c r="C16" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="17" spans="3:4">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3">
       <c r="C17" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="3:4">
+    <row r="18" spans="3:3">
       <c r="C18" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="19" spans="3:4">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3">
       <c r="C19" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="20" spans="3:4">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3">
       <c r="C20" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="21" spans="3:4">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3">
       <c r="C21" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="22" spans="3:4">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3">
       <c r="C22" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="23" spans="3:4">
       <c r="C23" s="2" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="24" spans="3:4">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="24" spans="3:3">
       <c r="C24" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="25" spans="3:4">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="25" spans="3:3">
       <c r="C25" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="26" spans="3:4">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="26" spans="3:3">
       <c r="C26" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="27" spans="3:4">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" spans="3:3">
       <c r="C27" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="28" spans="3:4">
+    <row r="28" spans="3:3">
       <c r="C28" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="3:4">
+    <row r="29" spans="3:3">
       <c r="C29" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="30" spans="3:4">
+    <row r="30" spans="3:3">
       <c r="C30" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="31" spans="3:4">
+    <row r="31" spans="3:3">
       <c r="C31" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="32" spans="3:4">
+    <row r="32" spans="3:3">
       <c r="C32" t="s">
         <v>341</v>
       </c>
@@ -5373,7 +5966,7 @@
     </row>
     <row r="41" spans="3:3">
       <c r="C41" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="42" spans="3:3">
@@ -5463,7 +6056,7 @@
     </row>
     <row r="59" spans="3:3">
       <c r="C59" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="60" spans="3:3">
@@ -5491,32 +6084,32 @@
         <v>371</v>
       </c>
     </row>
-    <row r="65" spans="3:4">
+    <row r="65" spans="3:3">
       <c r="C65" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="66" spans="3:4">
+    <row r="66" spans="3:3">
       <c r="C66" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="67" spans="3:4">
+    <row r="67" spans="3:3">
       <c r="C67" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="68" spans="3:4">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="68" spans="3:3">
       <c r="C68" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="69" spans="3:4">
+    <row r="69" spans="3:3">
       <c r="C69" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="70" spans="3:4">
+    <row r="70" spans="3:3">
       <c r="C70" t="s">
         <v>376</v>
       </c>
@@ -5526,10 +6119,10 @@
         <v>377</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="72" spans="3:4">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="72" spans="3:3">
       <c r="C72" t="s">
         <v>378</v>
       </c>
@@ -5539,25 +6132,25 @@
         <v>379</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="74" spans="3:4">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="74" spans="3:3">
       <c r="C74" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="75" spans="3:4">
+    <row r="75" spans="3:3">
       <c r="C75" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="76" spans="3:4">
+    <row r="76" spans="3:3">
       <c r="C76" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="77" spans="3:4">
+    <row r="77" spans="3:3">
       <c r="C77" t="s">
         <v>383</v>
       </c>
@@ -5567,7 +6160,7 @@
         <v>384</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="79" spans="3:4">
@@ -5575,10 +6168,10 @@
         <v>385</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="80" spans="3:4">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="80" spans="3:3">
       <c r="C80" t="s">
         <v>386</v>
       </c>
@@ -5665,7 +6258,7 @@
     </row>
     <row r="97" spans="3:3">
       <c r="C97" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="98" spans="3:3">
@@ -5690,12 +6283,13 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1">
       <formula1>$A$2:$A$12</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
   <tableParts count="2">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>

</xml_diff>

<commit_message>
CPR fund changes in prov and phar
adf
</commit_message>
<xml_diff>
--- a/QA/testcases/CPR/Pharmacy/Phar_Patient_App_Create_PCase_Positive.xlsx
+++ b/QA/testcases/CPR/Pharmacy/Phar_Patient_App_Create_PCase_Positive.xlsx
@@ -166,7 +166,7 @@
     <t>PATIENT_FUND_NAME</t>
   </si>
   <si>
-    <t>Breast Cancer Silo*</t>
+    <t>Hepatitis C***</t>
   </si>
   <si>
     <t>Enter fund name</t>
@@ -1245,10 +1245,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -1275,22 +1275,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1298,7 +1285,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1314,16 +1301,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1335,8 +1315,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1358,9 +1346,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1368,9 +1369,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1381,9 +1382,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1397,9 +1404,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1407,13 +1414,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1440,13 +1440,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1458,25 +1506,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1494,13 +1578,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1512,115 +1620,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1682,30 +1682,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1724,18 +1700,7 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1758,9 +1723,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1779,16 +1746,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1800,130 +1800,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2381,8 +2381,8 @@
   <sheetPr/>
   <dimension ref="A1:H156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85714285714286" defaultRowHeight="15" outlineLevelCol="7"/>

</xml_diff>